<commit_message>
Some Changes for presentation
</commit_message>
<xml_diff>
--- a/Product_Backlog.xlsx
+++ b/Product_Backlog.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB37C41-3CD7-4ABF-8C47-9EC80161ED95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B675C400-C0AD-49ED-A00B-7D3FAA426F52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3720" yWindow="1650" windowWidth="7500" windowHeight="6397" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3420" yWindow="3420" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="64">
   <si>
     <t>Nummer</t>
   </si>
@@ -215,6 +215,12 @@
   </si>
   <si>
     <t>D</t>
+  </si>
+  <si>
+    <t>2, 3</t>
+  </si>
+  <si>
+    <t>W</t>
   </si>
 </sst>
 </file>
@@ -250,14 +256,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -558,24 +567,24 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.796875" customWidth="1"/>
-    <col min="2" max="2" width="20.86328125" customWidth="1"/>
-    <col min="3" max="3" width="9.1328125" customWidth="1"/>
-    <col min="4" max="4" width="7.33203125" customWidth="1"/>
-    <col min="5" max="5" width="7.86328125" customWidth="1"/>
-    <col min="6" max="6" width="19.59765625" customWidth="1"/>
-    <col min="7" max="7" width="6.9296875" customWidth="1"/>
-    <col min="8" max="8" width="4" customWidth="1"/>
-    <col min="9" max="9" width="3.19921875" customWidth="1"/>
-    <col min="11" max="11" width="21.73046875" customWidth="1"/>
+    <col min="1" max="1" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="77.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -610,7 +619,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -635,11 +644,11 @@
       <c r="H2" t="s">
         <v>61</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -662,13 +671,13 @@
         <v>54</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3">
-        <v>2</v>
+        <v>63</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -691,13 +700,13 @@
         <v>54</v>
       </c>
       <c r="H4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4">
-        <v>2</v>
+        <v>63</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -720,13 +729,13 @@
         <v>55</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5">
-        <v>2</v>
+        <v>63</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -751,8 +760,9 @@
       <c r="H6" t="s">
         <v>15</v>
       </c>
+      <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -775,13 +785,13 @@
         <v>56</v>
       </c>
       <c r="H7" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7">
-        <v>2</v>
+        <v>63</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -806,8 +816,9 @@
       <c r="H8" t="s">
         <v>15</v>
       </c>
+      <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -832,8 +843,9 @@
       <c r="H9" t="s">
         <v>15</v>
       </c>
+      <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -858,8 +870,9 @@
       <c r="H10" t="s">
         <v>15</v>
       </c>
+      <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -884,8 +897,9 @@
       <c r="H11" t="s">
         <v>15</v>
       </c>
+      <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -910,6 +924,7 @@
       <c r="H12" t="s">
         <v>15</v>
       </c>
+      <c r="J12" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -920,15 +935,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100C2B765165B3DBC4EABCCAF9BDF2E9402" ma:contentTypeVersion="6" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="ff4c766c9ef51bc9b00dc70f3226a0aa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bdd5ea72-ad56-4e4f-b53b-7d88124ef7a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3e31698592f1fe758f408b607c172525" ns2:_="">
     <xsd:import namespace="bdd5ea72-ad56-4e4f-b53b-7d88124ef7a1"/>
@@ -1086,6 +1092,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1093,14 +1108,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{253760C6-6844-4B67-AC63-08B35197F0C6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C831619-75E7-4D20-912E-42A9D62847D0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1118,6 +1125,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{253760C6-6844-4B67-AC63-08B35197F0C6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0ED81832-FC5A-4594-A478-B4C5C58FF102}">
   <ds:schemaRefs>

</xml_diff>